<commit_message>
Added logic to handle different kinds of Configuration types. Surfaced a bug with reading Excel formula cells but the result of the formula is an empty string.
</commit_message>
<xml_diff>
--- a/src/test/resources/Personnel.xlsx
+++ b/src/test/resources/Personnel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t xml:space="preserve">ID Digits</t>
   </si>
@@ -40,6 +40,12 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Email Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newsletter Signup</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID Number</t>
   </si>
   <si>
@@ -52,6 +58,12 @@
     <t xml:space="preserve">Takahashi, Ryo</t>
   </si>
   <si>
+    <t xml:space="preserve">ryotakahashi@testgmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">05/18/80</t>
   </si>
   <si>
@@ -70,6 +82,9 @@
     <t xml:space="preserve">Urbosa, Menat-Darud</t>
   </si>
   <si>
+    <t xml:space="preserve">durbosa@testgmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">10/22/74</t>
   </si>
   <si>
@@ -88,6 +103,9 @@
     <t xml:space="preserve">Collins, Phil</t>
   </si>
   <si>
+    <t xml:space="preserve">therealphilcollins@testaol.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">02/30/02</t>
   </si>
   <si>
@@ -106,6 +124,12 @@
     <t xml:space="preserve">Collins, Cecille</t>
   </si>
   <si>
+    <t xml:space="preserve">cecille-collins@testtumblr.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
     <t xml:space="preserve">01/XX/99</t>
   </si>
   <si>
@@ -139,6 +163,9 @@
     <t xml:space="preserve">Dellany, Tammy</t>
   </si>
   <si>
+    <t xml:space="preserve">tamtam1988@testhotmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">TBD</t>
   </si>
   <si>
@@ -149,6 +176,30 @@
   </si>
   <si>
     <t xml:space="preserve">Under review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sapperstein, Donny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donsap@testgmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/01/14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blake, Kerry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kerryblake@testyahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/19/91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/11/12</t>
   </si>
 </sst>
 </file>
@@ -159,7 +210,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -188,12 +239,24 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -264,7 +327,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -289,10 +352,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -305,6 +376,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -313,8 +388,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -394,43 +473,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.4"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.4"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="2" t="s">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -442,72 +523,84 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="G2" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="H2" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="I2" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="3"/>
+      <c r="J2" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <f aca="false">_xlfn.CONCAT(D3:H3)</f>
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <f aca="false">_xlfn.CONCAT(F3:J3)</f>
         <v>55501</v>
       </c>
-      <c r="D3" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>5</v>
-      </c>
       <c r="F3" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G3" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="5" t="n">
+      <c r="J3" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>13</v>
+      <c r="K3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,41 +609,47 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="7" t="str">
-        <f aca="false">_xlfn.CONCAT(D4:H4)</f>
+        <v>19</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT(F4:J4)</f>
         <v>55502</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>5</v>
-      </c>
       <c r="F4" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>19</v>
+      <c r="K4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,41 +658,44 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="7" t="str">
-        <f aca="false">_xlfn.CONCAT(D5:H5)</f>
+        <v>26</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT(F5:J5)</f>
         <v>55503</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>5</v>
-      </c>
       <c r="F5" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="J5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>25</v>
+      <c r="K5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,75 +704,85 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT(F6:J6)</f>
+        <v>3940</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7" t="str">
-        <f aca="false">_xlfn.CONCAT(D6:H6)</f>
-        <v>3940</v>
-      </c>
-      <c r="D6" s="0" t="n">
+      <c r="D7" s="12"/>
+      <c r="E7" s="13" t="str">
+        <f aca="false">_xlfn.CONCAT(F7:J7)</f>
+        <v>55503</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="0" t="s">
+      <c r="K7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="0"/>
-      <c r="K6" s="0" t="s">
+      <c r="L7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="M7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="N7" s="11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="10" t="str">
-        <f aca="false">_xlfn.CONCAT(D7:H7)</f>
-        <v>55503</v>
-      </c>
-      <c r="D7" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="E7" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F7" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>26</v>
+      <c r="O7" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,57 +791,59 @@
         <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="7" t="str">
-        <f aca="false">_xlfn.CONCAT(D8:H8)</f>
+        <v>40</v>
+      </c>
+      <c r="E8" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT(F8:J8)</f>
         <v>00397</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="F8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="G8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="J8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="K8" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
+      <c r="A9" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -737,39 +851,134 @@
         <v>6</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="7" t="str">
-        <f aca="false">_xlfn.CONCAT(D10:H10)</f>
+        <v>46</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT(F10:J10)</f>
         <v>TBD</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>19</v>
+      <c r="F10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>42</v>
+        <v>23</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="16" t="n">
+        <f aca="false">A10+1</f>
+        <v>7</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT(F11:J11)</f>
+        <v>00629</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="16" t="n">
+        <f aca="false">A11+1</f>
+        <v>8</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT(F12:J12)</f>
+        <v/>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:N2"/>
-    <mergeCell ref="A9:N9"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:P2"/>
+    <mergeCell ref="A9:P9"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="ryotakahashi@testgmail.com"/>
+    <hyperlink ref="C4" r:id="rId2" display="durbosa@testgmail.com"/>
+    <hyperlink ref="C6" r:id="rId3" display="cecille-collins@testtumblr.com"/>
+    <hyperlink ref="C7" r:id="rId4" display="therealphilcollins@testaol.com"/>
+    <hyperlink ref="C10" r:id="rId5" display="tamtam1988@testhotmail.com"/>
+    <hyperlink ref="C11" r:id="rId6" display="donsap@testgmail.com"/>
+    <hyperlink ref="C12" r:id="rId7" display="kerryblake@testyahoo.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Fixed bug with reading Excel formula cell with blank results. Updated README.md.
</commit_message>
<xml_diff>
--- a/src/test/resources/Personnel.xlsx
+++ b/src/test/resources/Personnel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t xml:space="preserve">ID Digits</t>
   </si>
@@ -200,6 +200,18 @@
   </si>
   <si>
     <t xml:space="preserve">06/11/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two, Timbuk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timbuk2@testgmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/22/90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/29/15</t>
   </si>
 </sst>
 </file>
@@ -210,7 +222,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -252,11 +264,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -392,7 +399,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -473,7 +480,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -962,6 +969,43 @@
         <v>25</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="16" t="n">
+        <f aca="false">A12+1</f>
+        <v>9</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT(F13:J13)</f>
+        <v>7</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="F1:J1"/>
@@ -978,6 +1022,7 @@
     <hyperlink ref="C10" r:id="rId5" display="tamtam1988@testhotmail.com"/>
     <hyperlink ref="C11" r:id="rId6" display="donsap@testgmail.com"/>
     <hyperlink ref="C12" r:id="rId7" display="kerryblake@testyahoo.com"/>
+    <hyperlink ref="C13" r:id="rId8" display="timbuk2@testgmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>